<commit_message>
New datasets (updated bus schedule)
</commit_message>
<xml_diff>
--- a/data/FictitiousData.xlsx
+++ b/data/FictitiousData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachg\Documents\ug_thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E2195C-62AA-4C2E-A5FE-1E214781EFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D09C2C-F1BC-4446-8C3B-E9001121F4C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="799" activeTab="5" xr2:uid="{200E0D9B-9F6D-426A-BEB3-8930502E9E77}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="799" firstSheet="2" activeTab="5" xr2:uid="{200E0D9B-9F6D-426A-BEB3-8930502E9E77}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeWindows" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>TimeWindow</t>
   </si>
@@ -83,24 +83,6 @@
   </si>
   <si>
     <t>2 - Time</t>
-  </si>
-  <si>
-    <t>3 - Nodes</t>
-  </si>
-  <si>
-    <t>3 - Time</t>
-  </si>
-  <si>
-    <t>4 - Nodes</t>
-  </si>
-  <si>
-    <t>4 - Time</t>
-  </si>
-  <si>
-    <t>5 - Nodes</t>
-  </si>
-  <si>
-    <t>5 - Time</t>
   </si>
 </sst>
 </file>
@@ -3415,7 +3397,7 @@
   <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AB21" sqref="AB21"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5507,15 +5489,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93A33471-588E-4B24-8A7F-8A915BF72CF3}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -5528,1559 +5510,854 @@
       <c r="D1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="E2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <f>IF(B2="", "", IF(B2+VLOOKUP(PublicTransit!A2, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A3, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B2+VLOOKUP(PublicTransit!A2, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A3, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>2.6041666666666668E-2</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2">
+        <f>IF(D2="", "", IF(D2+VLOOKUP(PublicTransit!C2, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C3, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D2+VLOOKUP(PublicTransit!C2, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C3, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>8.6805555555555559E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <f>IF(B3="", "", IF(B3+VLOOKUP(PublicTransit!A3, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A4, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B3+VLOOKUP(PublicTransit!A3, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A4, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>6.0763888888888895E-2</v>
+      </c>
+      <c r="C4">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2">
+        <f>IF(D3="", "", IF(D3+VLOOKUP(PublicTransit!C3, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C4, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D3+VLOOKUP(PublicTransit!C3, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C4, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>4.3402777777777776E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>10</v>
       </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>15</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>21</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="B5" s="2">
+        <f>IF(B4="", "", IF(B4+VLOOKUP(PublicTransit!A4, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A5, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B4+VLOOKUP(PublicTransit!A4, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A5, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>8.6805555555555566E-2</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2">
+        <f>IF(D4="", "", IF(D4+VLOOKUP(PublicTransit!C4, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C5, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D4+VLOOKUP(PublicTransit!C4, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C5, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>6.0763888888888888E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2">
+        <f>IF(B5="", "", IF(B5+VLOOKUP(PublicTransit!A5, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A6, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B5+VLOOKUP(PublicTransit!A5, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A6, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.12152777777777779</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2">
+        <f>IF(D5="", "", IF(D5+VLOOKUP(PublicTransit!C5, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C6, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D5+VLOOKUP(PublicTransit!C5, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C6, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.10416666666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2">
+        <f>IF(B6="", "", IF(B6+VLOOKUP(PublicTransit!A6, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A7, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B6+VLOOKUP(PublicTransit!A6, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A7, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.14756944444444445</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2">
+        <f>IF(D6="", "", IF(D6+VLOOKUP(PublicTransit!C6, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C7, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D6+VLOOKUP(PublicTransit!C6, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C7, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.1388888888888889</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f>A2</f>
+        <v>20</v>
+      </c>
+      <c r="B8" s="2">
+        <f>IF(B7="", "", IF(B7+VLOOKUP(PublicTransit!A7, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A8, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B7+VLOOKUP(PublicTransit!A7, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A8, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.15625</v>
+      </c>
+      <c r="C8">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="E3">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G3">
+      <c r="D8" s="2">
+        <f>IF(D7="", "", IF(D7+VLOOKUP(PublicTransit!C7, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C8, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D7+VLOOKUP(PublicTransit!C7, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C8, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.19097222222222224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" ref="A9:A49" si="0">A3</f>
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
+        <f>IF(B8="", "", IF(B8+VLOOKUP(PublicTransit!A8, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A9, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B8+VLOOKUP(PublicTransit!A8, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A9, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.18229166666666666</v>
+      </c>
+      <c r="C9">
+        <f>C2</f>
+        <v>8</v>
+      </c>
+      <c r="D9" s="2">
+        <f>IF(D8="", "", IF(D8+VLOOKUP(PublicTransit!C8, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C9, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D8+VLOOKUP(PublicTransit!C8, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C9, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B10" s="2">
+        <f>IF(B9="", "", IF(B9+VLOOKUP(PublicTransit!A9, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A10, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B9+VLOOKUP(PublicTransit!A9, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A10, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.2170138888888889</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:C49" si="1">C3</f>
+        <v>9</v>
+      </c>
+      <c r="D10" s="2">
+        <f>IF(D9="", "", IF(D9+VLOOKUP(PublicTransit!C9, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C10, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D9+VLOOKUP(PublicTransit!C9, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C10, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.2170138888888889</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <f>IF(B10="", "", IF(B10+VLOOKUP(PublicTransit!A10, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A11, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B10+VLOOKUP(PublicTransit!A10, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A11, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="D11" s="2">
+        <f>IF(D10="", "", IF(D10+VLOOKUP(PublicTransit!C10, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C11, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D10+VLOOKUP(PublicTransit!C10, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C11, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.2517361111111111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B12" s="2">
+        <f>IF(B11="", "", IF(B11+VLOOKUP(PublicTransit!A11, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A12, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B11+VLOOKUP(PublicTransit!A11, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A12, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="D12" s="2">
+        <f>IF(D11="", "", IF(D11+VLOOKUP(PublicTransit!C11, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C12, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D11+VLOOKUP(PublicTransit!C11, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C12, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.26909722222222221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B13" s="2">
+        <f>IF(B12="", "", IF(B12+VLOOKUP(PublicTransit!A12, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A13, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B12+VLOOKUP(PublicTransit!A12, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A13, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.30381944444444448</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="H3" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="I3">
-        <v>22</v>
-      </c>
-      <c r="J3" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>4.1666666666666699E-2</v>
-      </c>
-      <c r="C4">
+      <c r="D13" s="2">
+        <f>IF(D12="", "", IF(D12+VLOOKUP(PublicTransit!C12, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C13, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D12+VLOOKUP(PublicTransit!C12, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C13, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B14" s="2">
+        <f>IF(B13="", "", IF(B13+VLOOKUP(PublicTransit!A13, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A14, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B13+VLOOKUP(PublicTransit!A13, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A14, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.31250000000000006</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="D14" s="2">
+        <f>IF(D13="", "", IF(D13+VLOOKUP(PublicTransit!C13, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C14, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D13+VLOOKUP(PublicTransit!C13, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C14, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.34722222222222221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B15" s="2">
+        <f>IF(B14="", "", IF(B14+VLOOKUP(PublicTransit!A14, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A15, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B14+VLOOKUP(PublicTransit!A14, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A15, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.33854166666666674</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D15" s="2">
+        <f>IF(D14="", "", IF(D14+VLOOKUP(PublicTransit!C14, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C15, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D14+VLOOKUP(PublicTransit!C14, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C15, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.39930555555555552</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D4" s="2">
-        <v>4.1666666666666699E-2</v>
-      </c>
-      <c r="E4">
+      <c r="B16" s="2">
+        <f>IF(B15="", "", IF(B15+VLOOKUP(PublicTransit!A15, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A16, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B15+VLOOKUP(PublicTransit!A15, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A16, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.37326388888888895</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D16" s="2">
+        <f>IF(D15="", "", IF(D15+VLOOKUP(PublicTransit!C15, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C16, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D15+VLOOKUP(PublicTransit!C15, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C16, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.41666666666666663</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B17" s="2">
+        <f>IF(B16="", "", IF(B16+VLOOKUP(PublicTransit!A16, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A17, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B16+VLOOKUP(PublicTransit!A16, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A17, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.39930555555555564</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D17" s="2">
+        <f>IF(D16="", "", IF(D16+VLOOKUP(PublicTransit!C16, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C17, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D16+VLOOKUP(PublicTransit!C16, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C17, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.42534722222222221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F4" s="2">
-        <v>4.1666666666666699E-2</v>
-      </c>
-      <c r="G4">
-        <v>17</v>
-      </c>
-      <c r="H4" s="2">
-        <v>4.1666666666666699E-2</v>
-      </c>
-      <c r="I4">
+      <c r="B18" s="2">
+        <f>IF(B17="", "", IF(B17+VLOOKUP(PublicTransit!A17, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A18, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B17+VLOOKUP(PublicTransit!A17, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A18, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.43402777777777785</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="J4" s="2">
-        <v>4.1666666666666699E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="C5">
+      <c r="D18" s="2">
+        <f>IF(D17="", "", IF(D17+VLOOKUP(PublicTransit!C17, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C18, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D17+VLOOKUP(PublicTransit!C17, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C18, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.46006944444444442</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B19" s="2">
+        <f>IF(B18="", "", IF(B18+VLOOKUP(PublicTransit!A18, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A19, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B18+VLOOKUP(PublicTransit!A18, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A19, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.46006944444444453</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="D19" s="2">
+        <f>IF(D18="", "", IF(D18+VLOOKUP(PublicTransit!C18, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C19, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D18+VLOOKUP(PublicTransit!C18, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C19, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.47743055555555552</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B20" s="2">
+        <f>IF(B19="", "", IF(B19+VLOOKUP(PublicTransit!A19, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A20, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B19+VLOOKUP(PublicTransit!A19, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A20, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.46875000000000011</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="D20" s="2">
+        <f>IF(D19="", "", IF(D19+VLOOKUP(PublicTransit!C19, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C20, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D19+VLOOKUP(PublicTransit!C19, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C20, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.52083333333333326</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B21" s="2">
+        <f>IF(B20="", "", IF(B20+VLOOKUP(PublicTransit!A20, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A21, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B20+VLOOKUP(PublicTransit!A20, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A21, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.4947916666666668</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="D21" s="2">
+        <f>IF(D20="", "", IF(D20+VLOOKUP(PublicTransit!C20, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C21, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D20+VLOOKUP(PublicTransit!C20, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C21, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.55555555555555547</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B22" s="2">
+        <f>IF(B21="", "", IF(B21+VLOOKUP(PublicTransit!A21, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A22, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B21+VLOOKUP(PublicTransit!A21, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A22, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.52951388888888906</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D22" s="2">
+        <f>IF(D21="", "", IF(D21+VLOOKUP(PublicTransit!C21, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C22, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D21+VLOOKUP(PublicTransit!C21, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C22, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.60763888888888884</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B23" s="2">
+        <f>IF(B22="", "", IF(B22+VLOOKUP(PublicTransit!A22, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A23, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B22+VLOOKUP(PublicTransit!A22, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A23, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.55555555555555569</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="D5" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E5">
-        <v>13</v>
-      </c>
-      <c r="F5" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="G5">
-        <v>18</v>
-      </c>
-      <c r="H5" s="2">
-        <v>6.25E-2</v>
-      </c>
-      <c r="I5">
+      <c r="D23" s="2">
+        <f>IF(D22="", "", IF(D22+VLOOKUP(PublicTransit!C22, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C23, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D22+VLOOKUP(PublicTransit!C22, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C23, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B24" s="2">
+        <f>IF(B23="", "", IF(B23+VLOOKUP(PublicTransit!A23, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A24, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B23+VLOOKUP(PublicTransit!A23, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A24, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.5902777777777779</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D24" s="2">
+        <f>IF(D23="", "", IF(D23+VLOOKUP(PublicTransit!C23, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C24, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D23+VLOOKUP(PublicTransit!C23, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C24, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.63368055555555558</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B25" s="2">
+        <f>IF(B24="", "", IF(B24+VLOOKUP(PublicTransit!A24, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A25, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B24+VLOOKUP(PublicTransit!A24, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A25, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.61631944444444453</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="D25" s="2">
+        <f>IF(D24="", "", IF(D24+VLOOKUP(PublicTransit!C24, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C25, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D24+VLOOKUP(PublicTransit!C24, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C25, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.66840277777777779</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B26" s="2">
+        <f>IF(B25="", "", IF(B25+VLOOKUP(PublicTransit!A25, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A26, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B25+VLOOKUP(PublicTransit!A25, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A26, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.62500000000000011</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="D26" s="2">
+        <f>IF(D25="", "", IF(D25+VLOOKUP(PublicTransit!C25, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C26, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D25+VLOOKUP(PublicTransit!C25, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C26, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.68576388888888895</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B27" s="2">
+        <f>IF(B26="", "", IF(B26+VLOOKUP(PublicTransit!A26, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A27, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B26+VLOOKUP(PublicTransit!A26, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A27, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.65104166666666674</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="D27" s="2">
+        <f>IF(D26="", "", IF(D26+VLOOKUP(PublicTransit!C26, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C27, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D26+VLOOKUP(PublicTransit!C26, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C27, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.72916666666666674</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B28" s="2">
+        <f>IF(B27="", "", IF(B27+VLOOKUP(PublicTransit!A27, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A28, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B27+VLOOKUP(PublicTransit!A27, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A28, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.68576388888888895</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="J5" s="2">
-        <v>6.25E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2">
-        <v>8.3333333333333301E-2</v>
-      </c>
-      <c r="C6">
+      <c r="D28" s="2">
+        <f>IF(D27="", "", IF(D27+VLOOKUP(PublicTransit!C27, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C28, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D27+VLOOKUP(PublicTransit!C27, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C28, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.76388888888888895</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B29" s="2">
+        <f>IF(B28="", "", IF(B28+VLOOKUP(PublicTransit!A28, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A29, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B28+VLOOKUP(PublicTransit!A28, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A29, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.71180555555555558</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D29" s="2">
+        <f>IF(D28="", "", IF(D28+VLOOKUP(PublicTransit!C28, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C29, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D28+VLOOKUP(PublicTransit!C28, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C29, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.81597222222222232</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B30" s="2">
+        <f>IF(B29="", "", IF(B29+VLOOKUP(PublicTransit!A29, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A30, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B29+VLOOKUP(PublicTransit!A29, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A30, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.74652777777777779</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D30" s="2">
+        <f>IF(D29="", "", IF(D29+VLOOKUP(PublicTransit!C29, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C30, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D29+VLOOKUP(PublicTransit!C29, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C30, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.83333333333333348</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B31" s="2">
+        <f>IF(B30="", "", IF(B30+VLOOKUP(PublicTransit!A30, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A31, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B30+VLOOKUP(PublicTransit!A30, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A31, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.77256944444444442</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="D6" s="2">
-        <v>8.3333333333333301E-2</v>
-      </c>
-      <c r="E6">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2">
-        <v>8.3333333333333301E-2</v>
-      </c>
-      <c r="G6">
+      <c r="D31" s="2">
+        <f>IF(D30="", "", IF(D30+VLOOKUP(PublicTransit!C30, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C31, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D30+VLOOKUP(PublicTransit!C30, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C31, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.84201388888888906</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B32" s="2">
+        <f>IF(B31="", "", IF(B31+VLOOKUP(PublicTransit!A31, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A32, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B31+VLOOKUP(PublicTransit!A31, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A32, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.78125</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="D32" s="2">
+        <f>IF(D31="", "", IF(D31+VLOOKUP(PublicTransit!C31, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C32, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D31+VLOOKUP(PublicTransit!C31, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C32, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.87673611111111127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B33" s="2">
+        <f>IF(B32="", "", IF(B32+VLOOKUP(PublicTransit!A32, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A33, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B32+VLOOKUP(PublicTransit!A32, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A33, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.80729166666666663</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="D33" s="2">
+        <f>IF(D32="", "", IF(D32+VLOOKUP(PublicTransit!C32, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C33, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D32+VLOOKUP(PublicTransit!C32, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C33, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.89409722222222243</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B34" s="2">
+        <f>IF(B33="", "", IF(B33+VLOOKUP(PublicTransit!A33, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A34, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B33+VLOOKUP(PublicTransit!A33, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A34, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.84201388888888884</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="D34" s="2">
+        <f>IF(D33="", "", IF(D33+VLOOKUP(PublicTransit!C33, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C34, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D33+VLOOKUP(PublicTransit!C33, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C34, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.93750000000000022</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B35" s="2">
+        <f>IF(B34="", "", IF(B34+VLOOKUP(PublicTransit!A34, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A35, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B34+VLOOKUP(PublicTransit!A34, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A35, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.86805555555555547</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="D35" s="2">
+        <f>IF(D34="", "", IF(D34+VLOOKUP(PublicTransit!C34, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C35, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D34+VLOOKUP(PublicTransit!C34, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C35, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.97222222222222243</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B36" s="2">
+        <f>IF(B35="", "", IF(B35+VLOOKUP(PublicTransit!A35, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A36, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B35+VLOOKUP(PublicTransit!A35, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A36, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.90277777777777768</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D36" s="2" t="str">
+        <f>IF(D35="", "", IF(D35+VLOOKUP(PublicTransit!C35, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C36, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D35+VLOOKUP(PublicTransit!C35, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C36, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="H6" s="2">
-        <v>8.3333333333333301E-2</v>
-      </c>
-      <c r="I6">
-        <v>25</v>
-      </c>
-      <c r="J6" s="2">
-        <v>8.3333333333333301E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="B37" s="2">
+        <f>IF(B36="", "", IF(B36+VLOOKUP(PublicTransit!A36, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A37, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B36+VLOOKUP(PublicTransit!A36, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A37, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.92881944444444431</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D37" s="2" t="str">
+        <f>IF(D36="", "", IF(D36+VLOOKUP(PublicTransit!C36, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C37, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D36+VLOOKUP(PublicTransit!C36, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C37, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B38" s="2">
+        <f>IF(B37="", "", IF(B37+VLOOKUP(PublicTransit!A37, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A38, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B37+VLOOKUP(PublicTransit!A37, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A38, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.93749999999999989</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D38" s="2" t="str">
+        <f>IF(D37="", "", IF(D37+VLOOKUP(PublicTransit!C37, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C38, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D37+VLOOKUP(PublicTransit!C37, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C38, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B39" s="2">
+        <f>IF(B38="", "", IF(B38+VLOOKUP(PublicTransit!A38, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A39, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B38+VLOOKUP(PublicTransit!A38, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A39, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.96354166666666652</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="D39" s="2" t="str">
+        <f>IF(D38="", "", IF(D38+VLOOKUP(PublicTransit!C38, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C39, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D38+VLOOKUP(PublicTransit!C38, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C39, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B40" s="2">
+        <f>IF(B39="", "", IF(B39+VLOOKUP(PublicTransit!A39, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A40, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B39+VLOOKUP(PublicTransit!A39, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A40, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v>0.99826388888888873</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="D40" s="2" t="str">
+        <f>IF(D39="", "", IF(D39+VLOOKUP(PublicTransit!C39, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C40, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D39+VLOOKUP(PublicTransit!C39, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C40, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B41" s="2" t="str">
+        <f>IF(B40="", "", IF(B40+VLOOKUP(PublicTransit!A40, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A41, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B40+VLOOKUP(PublicTransit!A40, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A41, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="D41" s="2" t="str">
+        <f>IF(D40="", "", IF(D40+VLOOKUP(PublicTransit!C40, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C41, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D40+VLOOKUP(PublicTransit!C40, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C41, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B42" s="2" t="str">
+        <f>IF(B41="", "", IF(B41+VLOOKUP(PublicTransit!A41, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A42, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B41+VLOOKUP(PublicTransit!A41, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A42, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="D42" s="2" t="str">
+        <f>IF(D41="", "", IF(D41+VLOOKUP(PublicTransit!C41, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C42, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D41+VLOOKUP(PublicTransit!C41, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C42, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B43" s="2" t="str">
+        <f>IF(B42="", "", IF(B42+VLOOKUP(PublicTransit!A42, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A43, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B42+VLOOKUP(PublicTransit!A42, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A43, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+      <c r="C43">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.104166666666667</v>
-      </c>
-      <c r="C7">
+      <c r="D43" s="2" t="str">
+        <f>IF(D42="", "", IF(D42+VLOOKUP(PublicTransit!C42, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C43, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D42+VLOOKUP(PublicTransit!C42, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C43, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B44" s="2" t="str">
+        <f>IF(B43="", "", IF(B43+VLOOKUP(PublicTransit!A43, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A44, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B43+VLOOKUP(PublicTransit!A43, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A44, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D44" s="2" t="str">
+        <f>IF(D43="", "", IF(D43+VLOOKUP(PublicTransit!C43, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C44, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D43+VLOOKUP(PublicTransit!C43, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C44, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D7" s="2">
-        <v>0.104166666666667</v>
-      </c>
-      <c r="E7">
+      <c r="B45" s="2" t="str">
+        <f>IF(B44="", "", IF(B44+VLOOKUP(PublicTransit!A44, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A45, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B44+VLOOKUP(PublicTransit!A44, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A45, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D45" s="2" t="str">
+        <f>IF(D44="", "", IF(D44+VLOOKUP(PublicTransit!C44, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C45, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D44+VLOOKUP(PublicTransit!C44, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C45, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B46" s="2" t="str">
+        <f>IF(B45="", "", IF(B45+VLOOKUP(PublicTransit!A45, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A46, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B45+VLOOKUP(PublicTransit!A45, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A46, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+      <c r="C46">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="D46" s="2" t="str">
+        <f>IF(D45="", "", IF(D45+VLOOKUP(PublicTransit!C45, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C46, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D45+VLOOKUP(PublicTransit!C45, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C46, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F7" s="2">
-        <v>0.104166666666667</v>
-      </c>
-      <c r="G7">
-        <v>20</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0.104166666666667</v>
-      </c>
-      <c r="I7">
-        <v>21</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0.104166666666667</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.125</v>
-      </c>
-      <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.125</v>
-      </c>
-      <c r="E8">
-        <v>11</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.125</v>
-      </c>
-      <c r="G8">
-        <v>15</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0.125</v>
-      </c>
-      <c r="I8">
-        <v>22</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.14583333333333301</v>
-      </c>
-      <c r="C9">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.14583333333333301</v>
-      </c>
-      <c r="E9">
+      <c r="B47" s="2" t="str">
+        <f>IF(B46="", "", IF(B46+VLOOKUP(PublicTransit!A46, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A47, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B46+VLOOKUP(PublicTransit!A46, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A47, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+      <c r="C47">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="D47" s="2" t="str">
+        <f>IF(D46="", "", IF(D46+VLOOKUP(PublicTransit!C46, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C47, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D46+VLOOKUP(PublicTransit!C46, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C47, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F9" s="2">
-        <v>0.14583333333333301</v>
-      </c>
-      <c r="G9">
+      <c r="B48" s="2" t="str">
+        <f>IF(B47="", "", IF(B47+VLOOKUP(PublicTransit!A47, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A48, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B47+VLOOKUP(PublicTransit!A47, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A48, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+      <c r="C48">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="H9" s="2">
-        <v>0.14583333333333301</v>
-      </c>
-      <c r="I9">
-        <v>23</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0.14583333333333301</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.16666666666666699</v>
-      </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.16666666666666699</v>
-      </c>
-      <c r="E10">
-        <v>13</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.16666666666666699</v>
-      </c>
-      <c r="G10">
-        <v>17</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0.16666666666666699</v>
-      </c>
-      <c r="I10">
+      <c r="D48" s="2" t="str">
+        <f>IF(D47="", "", IF(D47+VLOOKUP(PublicTransit!C47, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C48, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D47+VLOOKUP(PublicTransit!C47, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C48, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B49" s="2" t="str">
+        <f>IF(B48="", "", IF(B48+VLOOKUP(PublicTransit!A48, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A49, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", B48+VLOOKUP(PublicTransit!A48, 'OD-TravelTime'!$A$1:$Z$26, MATCH(A49, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
+      </c>
+      <c r="C49">
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="J10" s="2">
-        <v>0.16666666666666699</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0.1875</v>
-      </c>
-      <c r="C11">
-        <v>9</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.1875</v>
-      </c>
-      <c r="E11">
-        <v>14</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.1875</v>
-      </c>
-      <c r="G11">
-        <v>18</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0.1875</v>
-      </c>
-      <c r="I11">
-        <v>25</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0.1875</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.20833333333333301</v>
-      </c>
-      <c r="C12">
-        <v>5</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.20833333333333301</v>
-      </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0.20833333333333301</v>
-      </c>
-      <c r="G12">
-        <v>19</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0.20833333333333301</v>
-      </c>
-      <c r="I12">
-        <v>21</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0.20833333333333301</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0.22916666666666699</v>
-      </c>
-      <c r="C13">
-        <v>6</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0.22916666666666699</v>
-      </c>
-      <c r="E13">
-        <v>11</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0.22916666666666699</v>
-      </c>
-      <c r="G13">
-        <v>20</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0.22916666666666699</v>
-      </c>
-      <c r="I13">
-        <v>22</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0.22916666666666699</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="C14">
-        <v>7</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="E14">
-        <v>12</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="G14">
-        <v>15</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="I14">
-        <v>23</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0.27083333333333298</v>
-      </c>
-      <c r="C15">
-        <v>8</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.27083333333333298</v>
-      </c>
-      <c r="E15">
-        <v>13</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0.27083333333333298</v>
-      </c>
-      <c r="G15">
-        <v>16</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0.27083333333333298</v>
-      </c>
-      <c r="I15">
-        <v>24</v>
-      </c>
-      <c r="J15" s="2">
-        <v>0.27083333333333298</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>3</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="C16">
-        <v>9</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="E16">
-        <v>14</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="G16">
-        <v>17</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="I16">
-        <v>25</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0.29166666666666702</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>4</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0.3125</v>
-      </c>
-      <c r="C17">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.3125</v>
-      </c>
-      <c r="E17">
-        <v>10</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0.3125</v>
-      </c>
-      <c r="G17">
-        <v>18</v>
-      </c>
-      <c r="H17" s="2">
-        <v>0.3125</v>
-      </c>
-      <c r="I17">
-        <v>21</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0.3125</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="C18">
-        <v>6</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="E18">
-        <v>11</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="G18">
-        <v>19</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="I18">
-        <v>22</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0.33333333333333298</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0.35416666666666702</v>
-      </c>
-      <c r="C19">
-        <v>7</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0.35416666666666702</v>
-      </c>
-      <c r="E19">
-        <v>12</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0.35416666666666702</v>
-      </c>
-      <c r="G19">
-        <v>20</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0.35416666666666702</v>
-      </c>
-      <c r="I19">
-        <v>23</v>
-      </c>
-      <c r="J19" s="2">
-        <v>0.35416666666666702</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20" s="2">
-        <v>0.375</v>
-      </c>
-      <c r="C20">
-        <v>8</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.375</v>
-      </c>
-      <c r="E20">
-        <v>13</v>
-      </c>
-      <c r="F20" s="2">
-        <v>0.375</v>
-      </c>
-      <c r="G20">
-        <v>15</v>
-      </c>
-      <c r="H20" s="2">
-        <v>0.375</v>
-      </c>
-      <c r="I20">
-        <v>24</v>
-      </c>
-      <c r="J20" s="2">
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>4</v>
-      </c>
-      <c r="B21" s="2">
-        <v>0.39583333333333298</v>
-      </c>
-      <c r="C21">
-        <v>9</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.39583333333333298</v>
-      </c>
-      <c r="E21">
-        <v>14</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0.39583333333333298</v>
-      </c>
-      <c r="G21">
-        <v>16</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0.39583333333333298</v>
-      </c>
-      <c r="I21">
-        <v>25</v>
-      </c>
-      <c r="J21" s="2">
-        <v>0.39583333333333298</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22" s="2">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="C22">
-        <v>5</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="E22">
-        <v>10</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="G22">
-        <v>17</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="I22">
-        <v>21</v>
-      </c>
-      <c r="J22" s="2">
-        <v>0.41666666666666702</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>2</v>
-      </c>
-      <c r="B23" s="2">
-        <v>0.4375</v>
-      </c>
-      <c r="C23">
-        <v>6</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.4375</v>
-      </c>
-      <c r="E23">
-        <v>11</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0.4375</v>
-      </c>
-      <c r="G23">
-        <v>18</v>
-      </c>
-      <c r="H23" s="2">
-        <v>0.4375</v>
-      </c>
-      <c r="I23">
-        <v>22</v>
-      </c>
-      <c r="J23" s="2">
-        <v>0.4375</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>3</v>
-      </c>
-      <c r="B24" s="2">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="C24">
-        <v>7</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="E24">
-        <v>12</v>
-      </c>
-      <c r="F24" s="2">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="G24">
-        <v>19</v>
-      </c>
-      <c r="H24" s="2">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="I24">
-        <v>23</v>
-      </c>
-      <c r="J24" s="2">
-        <v>0.45833333333333298</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>4</v>
-      </c>
-      <c r="B25" s="2">
-        <v>0.47916666666666702</v>
-      </c>
-      <c r="C25">
-        <v>8</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.47916666666666702</v>
-      </c>
-      <c r="E25">
-        <v>13</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0.47916666666666702</v>
-      </c>
-      <c r="G25">
-        <v>20</v>
-      </c>
-      <c r="H25" s="2">
-        <v>0.47916666666666702</v>
-      </c>
-      <c r="I25">
-        <v>24</v>
-      </c>
-      <c r="J25" s="2">
-        <v>0.47916666666666702</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="C26">
-        <v>9</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E26">
-        <v>14</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="G26">
-        <v>15</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="I26">
-        <v>25</v>
-      </c>
-      <c r="J26" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>2</v>
-      </c>
-      <c r="B27" s="2">
-        <v>0.52083333333333304</v>
-      </c>
-      <c r="C27">
-        <v>5</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.52083333333333304</v>
-      </c>
-      <c r="E27">
-        <v>10</v>
-      </c>
-      <c r="F27" s="2">
-        <v>0.52083333333333304</v>
-      </c>
-      <c r="G27">
-        <v>16</v>
-      </c>
-      <c r="H27" s="2">
-        <v>0.52083333333333304</v>
-      </c>
-      <c r="I27">
-        <v>21</v>
-      </c>
-      <c r="J27" s="2">
-        <v>0.52083333333333304</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>3</v>
-      </c>
-      <c r="B28" s="2">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="C28">
-        <v>6</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="E28">
-        <v>11</v>
-      </c>
-      <c r="F28" s="2">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="G28">
-        <v>17</v>
-      </c>
-      <c r="H28" s="2">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="I28">
-        <v>22</v>
-      </c>
-      <c r="J28" s="2">
-        <v>0.54166666666666696</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>4</v>
-      </c>
-      <c r="B29" s="2">
-        <v>0.5625</v>
-      </c>
-      <c r="C29">
-        <v>7</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0.5625</v>
-      </c>
-      <c r="E29">
-        <v>12</v>
-      </c>
-      <c r="F29" s="2">
-        <v>0.5625</v>
-      </c>
-      <c r="G29">
-        <v>18</v>
-      </c>
-      <c r="H29" s="2">
-        <v>0.5625</v>
-      </c>
-      <c r="I29">
-        <v>23</v>
-      </c>
-      <c r="J29" s="2">
-        <v>0.5625</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30" s="2">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="C30">
-        <v>8</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="E30">
-        <v>13</v>
-      </c>
-      <c r="F30" s="2">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="G30">
-        <v>19</v>
-      </c>
-      <c r="H30" s="2">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="I30">
-        <v>24</v>
-      </c>
-      <c r="J30" s="2">
-        <v>0.58333333333333304</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>2</v>
-      </c>
-      <c r="B31" s="2">
-        <v>0.60416666666666696</v>
-      </c>
-      <c r="C31">
-        <v>9</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0.60416666666666696</v>
-      </c>
-      <c r="E31">
-        <v>14</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0.60416666666666696</v>
-      </c>
-      <c r="G31">
-        <v>20</v>
-      </c>
-      <c r="H31" s="2">
-        <v>0.60416666666666696</v>
-      </c>
-      <c r="I31">
-        <v>25</v>
-      </c>
-      <c r="J31" s="2">
-        <v>0.60416666666666696</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>3</v>
-      </c>
-      <c r="B32" s="2">
-        <v>0.625</v>
-      </c>
-      <c r="C32">
-        <v>5</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0.625</v>
-      </c>
-      <c r="E32">
-        <v>10</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0.625</v>
-      </c>
-      <c r="G32">
-        <v>15</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0.625</v>
-      </c>
-      <c r="I32">
-        <v>21</v>
-      </c>
-      <c r="J32" s="2">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>4</v>
-      </c>
-      <c r="B33" s="2">
-        <v>0.64583333333333304</v>
-      </c>
-      <c r="C33">
-        <v>6</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0.64583333333333304</v>
-      </c>
-      <c r="E33">
-        <v>11</v>
-      </c>
-      <c r="F33" s="2">
-        <v>0.64583333333333304</v>
-      </c>
-      <c r="G33">
-        <v>16</v>
-      </c>
-      <c r="H33" s="2">
-        <v>0.64583333333333304</v>
-      </c>
-      <c r="I33">
-        <v>22</v>
-      </c>
-      <c r="J33" s="2">
-        <v>0.64583333333333304</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>1</v>
-      </c>
-      <c r="B34" s="2">
-        <v>0.66666666666666696</v>
-      </c>
-      <c r="C34">
-        <v>7</v>
-      </c>
-      <c r="D34" s="2">
-        <v>0.66666666666666696</v>
-      </c>
-      <c r="E34">
-        <v>12</v>
-      </c>
-      <c r="F34" s="2">
-        <v>0.66666666666666696</v>
-      </c>
-      <c r="G34">
-        <v>17</v>
-      </c>
-      <c r="H34" s="2">
-        <v>0.66666666666666696</v>
-      </c>
-      <c r="I34">
-        <v>23</v>
-      </c>
-      <c r="J34" s="2">
-        <v>0.66666666666666696</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>2</v>
-      </c>
-      <c r="B35" s="2">
-        <v>0.6875</v>
-      </c>
-      <c r="C35">
-        <v>8</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0.6875</v>
-      </c>
-      <c r="E35">
-        <v>13</v>
-      </c>
-      <c r="F35" s="2">
-        <v>0.6875</v>
-      </c>
-      <c r="G35">
-        <v>18</v>
-      </c>
-      <c r="H35" s="2">
-        <v>0.6875</v>
-      </c>
-      <c r="I35">
-        <v>24</v>
-      </c>
-      <c r="J35" s="2">
-        <v>0.6875</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>3</v>
-      </c>
-      <c r="B36" s="2">
-        <v>0.70833333333333304</v>
-      </c>
-      <c r="C36">
-        <v>9</v>
-      </c>
-      <c r="D36" s="2">
-        <v>0.70833333333333304</v>
-      </c>
-      <c r="E36">
-        <v>14</v>
-      </c>
-      <c r="F36" s="2">
-        <v>0.70833333333333304</v>
-      </c>
-      <c r="G36">
-        <v>19</v>
-      </c>
-      <c r="H36" s="2">
-        <v>0.70833333333333304</v>
-      </c>
-      <c r="I36">
-        <v>25</v>
-      </c>
-      <c r="J36" s="2">
-        <v>0.70833333333333304</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>4</v>
-      </c>
-      <c r="B37" s="2">
-        <v>0.72916666666666696</v>
-      </c>
-      <c r="C37">
-        <v>5</v>
-      </c>
-      <c r="D37" s="2">
-        <v>0.72916666666666696</v>
-      </c>
-      <c r="E37">
-        <v>10</v>
-      </c>
-      <c r="F37" s="2">
-        <v>0.72916666666666696</v>
-      </c>
-      <c r="G37">
-        <v>20</v>
-      </c>
-      <c r="H37" s="2">
-        <v>0.72916666666666696</v>
-      </c>
-      <c r="I37">
-        <v>21</v>
-      </c>
-      <c r="J37" s="2">
-        <v>0.72916666666666696</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="C38">
-        <v>6</v>
-      </c>
-      <c r="D38" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="E38">
-        <v>11</v>
-      </c>
-      <c r="F38" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="G38">
-        <v>15</v>
-      </c>
-      <c r="H38" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="I38">
-        <v>22</v>
-      </c>
-      <c r="J38" s="2">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>2</v>
-      </c>
-      <c r="B39" s="2">
-        <v>0.77083333333333304</v>
-      </c>
-      <c r="C39">
-        <v>7</v>
-      </c>
-      <c r="D39" s="2">
-        <v>0.77083333333333304</v>
-      </c>
-      <c r="E39">
-        <v>12</v>
-      </c>
-      <c r="F39" s="2">
-        <v>0.77083333333333304</v>
-      </c>
-      <c r="G39">
-        <v>16</v>
-      </c>
-      <c r="H39" s="2">
-        <v>0.77083333333333304</v>
-      </c>
-      <c r="I39">
-        <v>23</v>
-      </c>
-      <c r="J39" s="2">
-        <v>0.77083333333333304</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>3</v>
-      </c>
-      <c r="B40" s="2">
-        <v>0.79166666666666696</v>
-      </c>
-      <c r="C40">
-        <v>8</v>
-      </c>
-      <c r="D40" s="2">
-        <v>0.79166666666666696</v>
-      </c>
-      <c r="E40">
-        <v>13</v>
-      </c>
-      <c r="F40" s="2">
-        <v>0.79166666666666696</v>
-      </c>
-      <c r="G40">
-        <v>17</v>
-      </c>
-      <c r="H40" s="2">
-        <v>0.79166666666666696</v>
-      </c>
-      <c r="I40">
-        <v>24</v>
-      </c>
-      <c r="J40" s="2">
-        <v>0.79166666666666696</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>4</v>
-      </c>
-      <c r="B41" s="2">
-        <v>0.8125</v>
-      </c>
-      <c r="C41">
-        <v>9</v>
-      </c>
-      <c r="D41" s="2">
-        <v>0.8125</v>
-      </c>
-      <c r="E41">
-        <v>14</v>
-      </c>
-      <c r="F41" s="2">
-        <v>0.8125</v>
-      </c>
-      <c r="G41">
-        <v>18</v>
-      </c>
-      <c r="H41" s="2">
-        <v>0.8125</v>
-      </c>
-      <c r="I41">
-        <v>25</v>
-      </c>
-      <c r="J41" s="2">
-        <v>0.8125</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>1</v>
-      </c>
-      <c r="B42" s="2">
-        <v>0.83333333333333304</v>
-      </c>
-      <c r="C42">
-        <v>5</v>
-      </c>
-      <c r="D42" s="2">
-        <v>0.83333333333333304</v>
-      </c>
-      <c r="E42">
-        <v>10</v>
-      </c>
-      <c r="F42" s="2">
-        <v>0.83333333333333304</v>
-      </c>
-      <c r="G42">
-        <v>19</v>
-      </c>
-      <c r="H42" s="2">
-        <v>0.83333333333333304</v>
-      </c>
-      <c r="I42">
-        <v>21</v>
-      </c>
-      <c r="J42" s="2">
-        <v>0.83333333333333304</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>2</v>
-      </c>
-      <c r="B43" s="2">
-        <v>0.85416666666666696</v>
-      </c>
-      <c r="C43">
-        <v>6</v>
-      </c>
-      <c r="D43" s="2">
-        <v>0.85416666666666696</v>
-      </c>
-      <c r="E43">
-        <v>11</v>
-      </c>
-      <c r="F43" s="2">
-        <v>0.85416666666666696</v>
-      </c>
-      <c r="G43">
-        <v>20</v>
-      </c>
-      <c r="H43" s="2">
-        <v>0.85416666666666696</v>
-      </c>
-      <c r="I43">
-        <v>22</v>
-      </c>
-      <c r="J43" s="2">
-        <v>0.85416666666666696</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>3</v>
-      </c>
-      <c r="B44" s="2">
-        <v>0.875</v>
-      </c>
-      <c r="C44">
-        <v>7</v>
-      </c>
-      <c r="D44" s="2">
-        <v>0.875</v>
-      </c>
-      <c r="E44">
-        <v>12</v>
-      </c>
-      <c r="F44" s="2">
-        <v>0.875</v>
-      </c>
-      <c r="G44">
-        <v>15</v>
-      </c>
-      <c r="H44" s="2">
-        <v>0.875</v>
-      </c>
-      <c r="I44">
-        <v>23</v>
-      </c>
-      <c r="J44" s="2">
-        <v>0.875</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>4</v>
-      </c>
-      <c r="B45" s="2">
-        <v>0.89583333333333304</v>
-      </c>
-      <c r="C45">
-        <v>8</v>
-      </c>
-      <c r="D45" s="2">
-        <v>0.89583333333333304</v>
-      </c>
-      <c r="E45">
-        <v>13</v>
-      </c>
-      <c r="F45" s="2">
-        <v>0.89583333333333304</v>
-      </c>
-      <c r="G45">
-        <v>16</v>
-      </c>
-      <c r="H45" s="2">
-        <v>0.89583333333333304</v>
-      </c>
-      <c r="I45">
-        <v>24</v>
-      </c>
-      <c r="J45" s="2">
-        <v>0.89583333333333304</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>1</v>
-      </c>
-      <c r="B46" s="2">
-        <v>0.91666666666666696</v>
-      </c>
-      <c r="C46">
-        <v>9</v>
-      </c>
-      <c r="D46" s="2">
-        <v>0.91666666666666696</v>
-      </c>
-      <c r="E46">
-        <v>14</v>
-      </c>
-      <c r="F46" s="2">
-        <v>0.91666666666666696</v>
-      </c>
-      <c r="G46">
-        <v>17</v>
-      </c>
-      <c r="H46" s="2">
-        <v>0.91666666666666696</v>
-      </c>
-      <c r="I46">
-        <v>25</v>
-      </c>
-      <c r="J46" s="2">
-        <v>0.91666666666666696</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>2</v>
-      </c>
-      <c r="B47" s="2">
-        <v>0.9375</v>
-      </c>
-      <c r="C47">
-        <v>5</v>
-      </c>
-      <c r="D47" s="2">
-        <v>0.9375</v>
-      </c>
-      <c r="E47">
-        <v>10</v>
-      </c>
-      <c r="F47" s="2">
-        <v>0.9375</v>
-      </c>
-      <c r="G47">
-        <v>18</v>
-      </c>
-      <c r="H47" s="2">
-        <v>0.9375</v>
-      </c>
-      <c r="I47">
-        <v>21</v>
-      </c>
-      <c r="J47" s="2">
-        <v>0.9375</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>3</v>
-      </c>
-      <c r="B48" s="2">
-        <v>0.95833333333333304</v>
-      </c>
-      <c r="C48">
-        <v>6</v>
-      </c>
-      <c r="D48" s="2">
-        <v>0.95833333333333304</v>
-      </c>
-      <c r="E48">
-        <v>11</v>
-      </c>
-      <c r="F48" s="2">
-        <v>0.95833333333333304</v>
-      </c>
-      <c r="G48">
-        <v>19</v>
-      </c>
-      <c r="H48" s="2">
-        <v>0.95833333333333304</v>
-      </c>
-      <c r="I48">
-        <v>22</v>
-      </c>
-      <c r="J48" s="2">
-        <v>0.95833333333333304</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>4</v>
-      </c>
-      <c r="B49" s="2">
-        <v>0.97916666666666696</v>
-      </c>
-      <c r="C49">
-        <v>7</v>
-      </c>
-      <c r="D49" s="2">
-        <v>0.97916666666666696</v>
-      </c>
-      <c r="E49">
-        <v>12</v>
-      </c>
-      <c r="F49" s="2">
-        <v>0.97916666666666696</v>
-      </c>
-      <c r="G49">
-        <v>20</v>
-      </c>
-      <c r="H49" s="2">
-        <v>0.97916666666666696</v>
-      </c>
-      <c r="I49">
-        <v>23</v>
-      </c>
-      <c r="J49" s="2">
-        <v>0.97916666666666696</v>
+      <c r="D49" s="2" t="str">
+        <f>IF(D48="", "", IF(D48+VLOOKUP(PublicTransit!C48, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C49, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60&gt;1, "", D48+VLOOKUP(PublicTransit!C48, 'OD-TravelTime'!$A$1:$Z$26, MATCH(C49, 'OD-TravelTime'!$B$1:$Z$1)+1)/24/60))</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>